<commit_message>
latest commit on 06/02/2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
+++ b/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9024" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9024" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Messages" sheetId="3" r:id="rId3"/>
+    <sheet name="Tickets" sheetId="4" r:id="rId4"/>
+    <sheet name="Projects" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Title</t>
   </si>
@@ -53,7 +56,7 @@
     <t>Kerala</t>
   </si>
   <si>
-    <t>Test label By APS</t>
+    <t>test_APS</t>
   </si>
   <si>
     <t>APS Company</t>
@@ -111,6 +114,78 @@
   </si>
   <si>
     <t>xyz aps group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To </t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Saumia Alex</t>
+  </si>
+  <si>
+    <t>This is a test subject from APS</t>
+  </si>
+  <si>
+    <t>Hi, Saumia . This is test message from APS</t>
+  </si>
+  <si>
+    <t>D:\Selenium\Steps_QALegendCRM.pdf</t>
+  </si>
+  <si>
+    <t>Ticket Type</t>
+  </si>
+  <si>
+    <t>Assign to</t>
+  </si>
+  <si>
+    <t>Test ticket APS</t>
+  </si>
+  <si>
+    <t>General support</t>
+  </si>
+  <si>
+    <t>This is a test ticket from APS</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>DeadLine</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>TestProject</t>
+  </si>
+  <si>
+    <t>Test projectby APS</t>
+  </si>
+  <si>
+    <t>testLabel by APS</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>1,6</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1137,8 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1139,7 +1214,7 @@
   <sheetPr/>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1158,7 +1233,7 @@
     <col min="12" max="12" width="17.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="23" customHeight="1" spans="1:12">
+    <row r="1" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1226,6 +1301,197 @@
       </c>
       <c r="J2" t="s">
         <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="11.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="26.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="36.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="42.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="14.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="17.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="15.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="24.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="12.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="18.7777777777778" customWidth="1"/>
+    <col min="7" max="7" width="19.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest commit on 10/02/2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
+++ b/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
@@ -4,21 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="9024" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
     <sheet name="Messages" sheetId="3" r:id="rId3"/>
-    <sheet name="Tickets" sheetId="4" r:id="rId4"/>
-    <sheet name="Projects" sheetId="5" r:id="rId5"/>
+    <sheet name="LoginData" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="Tickets" sheetId="4" r:id="rId6"/>
+    <sheet name="Projects" sheetId="5" r:id="rId7"/>
+    <sheet name="Notes" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Title</t>
   </si>
@@ -92,10 +95,7 @@
     <t>Client Groups</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>CurrencySymbol</t>
+    <t>Download location</t>
   </si>
   <si>
     <t>APS Test Company</t>
@@ -131,7 +131,7 @@
     <t>Saumia Alex</t>
   </si>
   <si>
-    <t>This is a test subject from APS</t>
+    <t xml:space="preserve"> APS -This is a test subject from APS</t>
   </si>
   <si>
     <t>Hi, Saumia . This is test message from APS</t>
@@ -140,6 +140,18 @@
     <t>D:\Selenium\Steps_QALegendCRM.pdf</t>
   </si>
   <si>
+    <t xml:space="preserve">Username </t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin@admin.Com</t>
+  </si>
+  <si>
+    <t>admin@adminInvalid.Com</t>
+  </si>
+  <si>
     <t>Ticket Type</t>
   </si>
   <si>
@@ -186,6 +198,9 @@
   </si>
   <si>
     <t>1,6</t>
+  </si>
+  <si>
+    <t>A new Title</t>
   </si>
 </sst>
 </file>
@@ -199,7 +214,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,9 +233,17 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -678,140 +701,140 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1152,31 +1175,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1215,7 +1238,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1233,53 +1256,50 @@
     <col min="12" max="12" width="17.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" ht="22.95" customHeight="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1288,19 +1308,19 @@
         <v>654321</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <v>9876896552</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2">
         <v>5467782</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1335,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1327,31 +1347,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1361,6 +1381,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="18.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="15.1111111111111" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>12345600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="admin@admin.Com"/>
+    <hyperlink ref="A3" r:id="rId1" display="admin@admin.Com"/>
+    <hyperlink ref="A4" r:id="rId2" display="admin@adminInvalid.Com" tooltip="mailto:admin@adminInvalid.Com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F2"/>
@@ -1378,41 +1472,41 @@
     <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1424,12 +1518,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1441,57 +1535,87 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="14.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All running test cases. Commit on 13/02/2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
+++ b/QA_Legend/src/main/java/TestData/TestData_Excel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FFC4F134-AE26-4B9A-B47B-6D9995F49E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,8 @@
     <sheet name="Projects" sheetId="5" r:id="rId7"/>
     <sheet name="Notes" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N23"/>
 </workbook>
 </file>
 
@@ -206,15 +208,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,338 +241,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -585,316 +258,34 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1152,26 +543,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="23.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="12.2222222222222" customWidth="1"/>
-    <col min="6" max="6" width="26.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1203,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="28.8" spans="1:7">
+    <row r="2" spans="1:9" ht="28.8">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1228,35 +619,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="16.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="16.4444444444444" customWidth="1"/>
-    <col min="4" max="4" width="14.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="11.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="7.77777777777778" customWidth="1"/>
-    <col min="7" max="7" width="11.7777777777778"/>
-    <col min="8" max="8" width="18.4444444444444" customWidth="1"/>
-    <col min="9" max="9" width="12.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="11.5555555555556" customWidth="1"/>
-    <col min="12" max="12" width="17.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="22.95" customHeight="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="22.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +680,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1325,25 +714,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="26.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="36.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="42.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1376,23 +763,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="15.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1429,18 +814,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="admin@admin.Com"/>
-    <hyperlink ref="A3" r:id="rId1" display="admin@admin.Com"/>
-    <hyperlink ref="A4" r:id="rId2" display="admin@adminInvalid.Com" tooltip="mailto:admin@adminInvalid.Com"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="mailto:admin@adminInvalid.Com" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1450,29 +833,27 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="17.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="15.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="24.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1514,27 +895,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="18.7777777777778" customWidth="1"/>
-    <col min="7" max="7" width="19.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1590,22 +967,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1620,6 +995,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>